<commit_message>
Segundo commit: cargar df a tabla
</commit_message>
<xml_diff>
--- a/DCVG_PPM_T_LBBR_10_24_1300010947_551003090_TEL_Rev0.xlsx
+++ b/DCVG_PPM_T_LBBR_10_24_1300010947_551003090_TEL_Rev0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Requerimientos\TGI\AUTOMATIZACION_CARGUE_UPDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED0094A-B656-4C9A-8571-FEEB89AF00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8D8BB5-4DC0-4D46-B205-3C5382FF274B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1558,9 +1558,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="168" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1657,7 +1659,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1711,6 +1713,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Énfasis1 2 7" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2033,7 +2044,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2042,7 +2053,7 @@
     <col min="2" max="3" width="11.33203125" style="3"/>
     <col min="4" max="4" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3"/>
     <col min="9" max="9" width="14.33203125" style="12" customWidth="1"/>
@@ -2145,7 +2156,7 @@
       <c r="E2" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="19">
         <v>45576</v>
       </c>
       <c r="G2" s="9">
@@ -2195,7 +2206,7 @@
       <c r="E3" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="20">
         <v>45576</v>
       </c>
       <c r="G3" s="9">
@@ -2249,7 +2260,7 @@
       <c r="E4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="21">
         <v>45576</v>
       </c>
       <c r="G4" s="9">

</xml_diff>

<commit_message>
Tercer commit: ajuste json y validaciones3
</commit_message>
<xml_diff>
--- a/DCVG_PPM_T_LBBR_10_24_1300010947_551003090_TEL_Rev0.xlsx
+++ b/DCVG_PPM_T_LBBR_10_24_1300010947_551003090_TEL_Rev0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Requerimientos\TGI\AUTOMATIZACION_CARGUE_UPDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8D8BB5-4DC0-4D46-B205-3C5382FF274B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9216836-30A0-481B-9382-E4A00BAFF9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCVG" sheetId="1" r:id="rId1"/>
@@ -1558,11 +1558,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="168" formatCode="[$-240A]dddd\,\ dd&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1659,7 +1658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1713,13 +1712,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2044,7 +2037,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2088,7 +2081,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2156,7 +2149,7 @@
       <c r="E2" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="6">
         <v>45576</v>
       </c>
       <c r="G2" s="9">
@@ -2206,7 +2199,7 @@
       <c r="E3" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="6">
         <v>45576</v>
       </c>
       <c r="G3" s="9">
@@ -2260,7 +2253,7 @@
       <c r="E4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="6">
         <v>45576</v>
       </c>
       <c r="G4" s="9">
@@ -3067,7 +3060,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>503</v>
       </c>
@@ -3169,7 +3162,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>503</v>
       </c>
@@ -3319,7 +3312,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>503</v>
       </c>

</xml_diff>